<commit_message>
small fixes to the metrics documentation
</commit_message>
<xml_diff>
--- a/docs/docs/metrics.xlsx
+++ b/docs/docs/metrics.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="282">
   <si>
     <t>Metrics</t>
   </si>
@@ -912,12 +912,106 @@
   <si>
     <t>Id</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> set consists of metrics with respect to which the mean of benign benchmark apps and that of malicious benchmark apps differ by at least 2% (i.e., </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>noticeably different</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">D </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">set consists of metrics with respect to which the mean of benign benchmark apps and that of malicious benchmark apps differ by at least 5% (i.e., </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>disparately different</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1035,6 +1129,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1050,7 +1152,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1184,11 +1286,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1212,9 +1323,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1264,6 +1372,13 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1572,10 +1687,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B2:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1594,7 +1712,7 @@
       </c>
     </row>
     <row r="3" spans="2:3" ht="21.75" customHeight="1" thickBot="1">
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="8"/>
@@ -1648,16 +1766,16 @@
       </c>
     </row>
     <row r="10" spans="2:3" ht="21.75" customHeight="1" thickBot="1">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="11"/>
     </row>
     <row r="11" spans="2:3" ht="30.75" thickTop="1">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1670,10 +1788,10 @@
       </c>
     </row>
     <row r="13" spans="2:3" ht="20.25" customHeight="1" thickBot="1">
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="11"/>
     </row>
     <row r="14" spans="2:3" ht="60.75" thickTop="1">
       <c r="B14" s="4" t="s">
@@ -1709,17 +1827,20 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G124"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="B133" sqref="B133"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1731,1960 +1852,1994 @@
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7">
-      <c r="B2" s="13" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="27" t="s">
+        <v>280</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="B4" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C4" s="21" t="s">
         <v>279</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="15.75">
-      <c r="B3" s="27" t="s">
+    <row r="5" spans="1:8" ht="15.75">
+      <c r="B5" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C5" s="20">
         <v>1</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D5" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E5" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="26.25">
-      <c r="B4" s="27"/>
-      <c r="C4" s="21">
+      <c r="F5" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="26.25">
+      <c r="B6" s="29"/>
+      <c r="C6" s="20">
         <v>2</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E6" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="F4" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="15.75">
-      <c r="B5" s="27"/>
-      <c r="C5" s="21">
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="B7" s="29"/>
+      <c r="C7" s="20">
         <v>3</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D7" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="F5" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="26.25">
-      <c r="B6" s="27"/>
-      <c r="C6" s="21">
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+    </row>
+    <row r="8" spans="1:8" ht="26.25">
+      <c r="B8" s="29"/>
+      <c r="C8" s="20">
         <v>4</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D8" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E8" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-    </row>
-    <row r="7" spans="2:7" ht="26.25">
-      <c r="B7" s="27"/>
-      <c r="C7" s="21">
+      <c r="F8" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="26.25">
+      <c r="B9" s="29"/>
+      <c r="C9" s="20">
         <v>5</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D9" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E9" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-    </row>
-    <row r="8" spans="2:7" ht="26.25">
-      <c r="B8" s="27"/>
-      <c r="C8" s="21">
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" spans="1:8" ht="26.25">
+      <c r="B10" s="29"/>
+      <c r="C10" s="20">
         <v>6</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D10" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E10" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-    </row>
-    <row r="9" spans="2:7">
-      <c r="B9" s="27"/>
-      <c r="C9" s="21">
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75">
+      <c r="B11" s="29"/>
+      <c r="C11" s="20">
         <v>7</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D11" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E11" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-    </row>
-    <row r="10" spans="2:7" ht="26.25">
-      <c r="B10" s="27"/>
-      <c r="C10" s="21">
+      <c r="F11" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="26.25">
+      <c r="B12" s="29"/>
+      <c r="C12" s="20">
         <v>8</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D12" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E12" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-    </row>
-    <row r="11" spans="2:7" ht="26.25">
-      <c r="B11" s="27"/>
-      <c r="C11" s="21">
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+    </row>
+    <row r="13" spans="1:8" ht="26.25">
+      <c r="B13" s="29"/>
+      <c r="C13" s="20">
         <v>9</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D13" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E13" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-    </row>
-    <row r="12" spans="2:7" ht="39">
-      <c r="B12" s="27"/>
-      <c r="C12" s="21">
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="1:8" ht="39">
+      <c r="B14" s="29"/>
+      <c r="C14" s="20">
         <v>10</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E14" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="F12" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="39">
-      <c r="B13" s="27"/>
-      <c r="C13" s="21">
+      <c r="F14" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="39">
+      <c r="B15" s="29"/>
+      <c r="C15" s="20">
         <v>11</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D15" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E15" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="F13" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G13" s="18"/>
-    </row>
-    <row r="14" spans="2:7" ht="39">
-      <c r="B14" s="27"/>
-      <c r="C14" s="21">
+      <c r="F15" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="1:8" ht="39">
+      <c r="B16" s="29"/>
+      <c r="C16" s="20">
         <v>12</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D16" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E16" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="F14" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G14" s="18"/>
-    </row>
-    <row r="15" spans="2:7" ht="39">
-      <c r="B15" s="27"/>
-      <c r="C15" s="21">
+      <c r="F16" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="2:7" ht="39">
+      <c r="B17" s="29"/>
+      <c r="C17" s="20">
         <v>13</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D17" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E17" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="F15" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="39">
-      <c r="B16" s="27"/>
-      <c r="C16" s="21">
+      <c r="F17" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="39">
+      <c r="B18" s="29"/>
+      <c r="C18" s="20">
         <v>14</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D18" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E18" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="F16" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G16" s="18"/>
-    </row>
-    <row r="17" spans="2:7" ht="39">
-      <c r="B17" s="27"/>
-      <c r="C17" s="21">
+      <c r="F18" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G18" s="17"/>
+    </row>
+    <row r="19" spans="2:7" ht="39">
+      <c r="B19" s="29"/>
+      <c r="C19" s="20">
         <v>15</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D19" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E19" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="F17" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G17" s="18"/>
-    </row>
-    <row r="18" spans="2:7" ht="39">
-      <c r="B18" s="27"/>
-      <c r="C18" s="21">
+      <c r="F19" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G19" s="17"/>
+    </row>
+    <row r="20" spans="2:7" ht="39">
+      <c r="B20" s="29"/>
+      <c r="C20" s="20">
         <v>16</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D20" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E20" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="F18" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="39">
-      <c r="B19" s="27"/>
-      <c r="C19" s="21">
+      <c r="F20" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="39">
+      <c r="B21" s="29"/>
+      <c r="C21" s="20">
         <v>17</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D21" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E21" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-    </row>
-    <row r="20" spans="2:7" ht="39">
-      <c r="B20" s="27"/>
-      <c r="C20" s="21">
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+    </row>
+    <row r="22" spans="2:7" ht="39">
+      <c r="B22" s="29"/>
+      <c r="C22" s="20">
         <v>18</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D22" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E22" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-    </row>
-    <row r="21" spans="2:7" ht="39">
-      <c r="B21" s="27"/>
-      <c r="C21" s="21">
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+    </row>
+    <row r="23" spans="2:7" ht="39">
+      <c r="B23" s="29"/>
+      <c r="C23" s="20">
         <v>19</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D23" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E23" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="F21" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="39">
-      <c r="B22" s="27"/>
-      <c r="C22" s="21">
+      <c r="F23" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="39">
+      <c r="B24" s="29"/>
+      <c r="C24" s="20">
         <v>20</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D24" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E24" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-    </row>
-    <row r="23" spans="2:7" ht="39">
-      <c r="B23" s="27"/>
-      <c r="C23" s="21">
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+    </row>
+    <row r="25" spans="2:7" ht="39">
+      <c r="B25" s="29"/>
+      <c r="C25" s="20">
         <v>21</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D25" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E25" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-    </row>
-    <row r="24" spans="2:7" ht="39">
-      <c r="B24" s="27"/>
-      <c r="C24" s="21">
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+    </row>
+    <row r="26" spans="2:7" ht="39">
+      <c r="B26" s="29"/>
+      <c r="C26" s="20">
         <v>22</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D26" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E26" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="F24" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G24" s="18"/>
-    </row>
-    <row r="25" spans="2:7" ht="39">
-      <c r="B25" s="27"/>
-      <c r="C25" s="21">
+      <c r="F26" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G26" s="17"/>
+    </row>
+    <row r="27" spans="2:7" ht="39">
+      <c r="B27" s="29"/>
+      <c r="C27" s="20">
         <v>23</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D27" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E27" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="F25" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G25" s="18"/>
-    </row>
-    <row r="26" spans="2:7" ht="39">
-      <c r="B26" s="27"/>
-      <c r="C26" s="21">
+      <c r="F27" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G27" s="17"/>
+    </row>
+    <row r="28" spans="2:7" ht="39">
+      <c r="B28" s="29"/>
+      <c r="C28" s="20">
         <v>24</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D28" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="E28" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="F26" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G26" s="18"/>
-    </row>
-    <row r="27" spans="2:7" ht="39">
-      <c r="B27" s="27"/>
-      <c r="C27" s="21">
+      <c r="F28" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G28" s="17"/>
+    </row>
+    <row r="29" spans="2:7" ht="39">
+      <c r="B29" s="29"/>
+      <c r="C29" s="20">
         <v>25</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D29" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E29" s="14" t="s">
         <v>230</v>
       </c>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-    </row>
-    <row r="28" spans="2:7" ht="39">
-      <c r="B28" s="27"/>
-      <c r="C28" s="21">
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+    </row>
+    <row r="30" spans="2:7" ht="39">
+      <c r="B30" s="29"/>
+      <c r="C30" s="20">
         <v>26</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D30" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="E30" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-    </row>
-    <row r="29" spans="2:7" ht="39">
-      <c r="B29" s="27"/>
-      <c r="C29" s="21">
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+    </row>
+    <row r="31" spans="2:7" ht="39">
+      <c r="B31" s="29"/>
+      <c r="C31" s="20">
         <v>27</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D31" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E31" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-    </row>
-    <row r="30" spans="2:7" ht="39">
-      <c r="B30" s="27"/>
-      <c r="C30" s="21">
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+    </row>
+    <row r="32" spans="2:7" ht="39">
+      <c r="B32" s="29"/>
+      <c r="C32" s="20">
         <v>28</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D32" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E32" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="F30" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G30" s="18"/>
-    </row>
-    <row r="31" spans="2:7" ht="39">
-      <c r="B31" s="27"/>
-      <c r="C31" s="21">
+      <c r="F32" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G32" s="17"/>
+    </row>
+    <row r="33" spans="2:7" ht="39">
+      <c r="B33" s="29"/>
+      <c r="C33" s="20">
         <v>29</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D33" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="E33" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-    </row>
-    <row r="32" spans="2:7" ht="39">
-      <c r="B32" s="27"/>
-      <c r="C32" s="21">
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+    </row>
+    <row r="34" spans="2:7" ht="39">
+      <c r="B34" s="29"/>
+      <c r="C34" s="20">
         <v>30</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D34" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E34" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-    </row>
-    <row r="33" spans="2:7" ht="39">
-      <c r="B33" s="27"/>
-      <c r="C33" s="21">
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+    </row>
+    <row r="35" spans="2:7" ht="39">
+      <c r="B35" s="29"/>
+      <c r="C35" s="20">
         <v>31</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D35" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E35" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-    </row>
-    <row r="34" spans="2:7" ht="39">
-      <c r="B34" s="27"/>
-      <c r="C34" s="21">
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+    </row>
+    <row r="36" spans="2:7" ht="39">
+      <c r="B36" s="29"/>
+      <c r="C36" s="20">
         <v>32</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D36" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E36" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-    </row>
-    <row r="35" spans="2:7" ht="39">
-      <c r="B35" s="27"/>
-      <c r="C35" s="21">
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+    </row>
+    <row r="37" spans="2:7" ht="39">
+      <c r="B37" s="29"/>
+      <c r="C37" s="20">
         <v>33</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D37" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="E37" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-    </row>
-    <row r="36" spans="2:7" ht="51.75">
-      <c r="B36" s="27"/>
-      <c r="C36" s="21">
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+    </row>
+    <row r="38" spans="2:7" ht="51.75">
+      <c r="B38" s="29"/>
+      <c r="C38" s="20">
         <v>34</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D38" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="E36" s="15" t="s">
+      <c r="E38" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="F36" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G36" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" ht="51.75">
-      <c r="B37" s="27"/>
-      <c r="C37" s="21">
+      <c r="F38" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G38" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="51.75">
+      <c r="B39" s="29"/>
+      <c r="C39" s="20">
         <v>35</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D39" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="E37" s="15" t="s">
+      <c r="E39" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="F37" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G37" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" ht="51.75">
-      <c r="B38" s="27"/>
-      <c r="C38" s="21">
+      <c r="F39" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G39" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="51.75">
+      <c r="B40" s="29"/>
+      <c r="C40" s="20">
         <v>36</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D40" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="E40" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="F38" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G38" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" ht="51.75">
-      <c r="B39" s="27"/>
-      <c r="C39" s="21">
+      <c r="F40" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G40" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="51.75">
+      <c r="B41" s="29"/>
+      <c r="C41" s="20">
         <v>37</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="D41" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="E39" s="15" t="s">
+      <c r="E41" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="F39" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G39" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" ht="51.75">
-      <c r="B40" s="27"/>
-      <c r="C40" s="21">
+      <c r="F41" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G41" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="51.75">
+      <c r="B42" s="29"/>
+      <c r="C42" s="20">
         <v>38</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D42" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="E40" s="15" t="s">
+      <c r="E42" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-    </row>
-    <row r="41" spans="2:7" ht="51.75">
-      <c r="B41" s="27"/>
-      <c r="C41" s="21">
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+    </row>
+    <row r="43" spans="2:7" ht="51.75">
+      <c r="B43" s="29"/>
+      <c r="C43" s="20">
         <v>39</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D43" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="E41" s="15" t="s">
+      <c r="E43" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-    </row>
-    <row r="42" spans="2:7" ht="51.75">
-      <c r="B42" s="27"/>
-      <c r="C42" s="21">
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+    </row>
+    <row r="44" spans="2:7" ht="51.75">
+      <c r="B44" s="29"/>
+      <c r="C44" s="20">
         <v>40</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D44" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="E42" s="15" t="s">
+      <c r="E44" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="F42" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G42" s="18"/>
-    </row>
-    <row r="43" spans="2:7" ht="51.75">
-      <c r="B43" s="27"/>
-      <c r="C43" s="21">
+      <c r="F44" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G44" s="17"/>
+    </row>
+    <row r="45" spans="2:7" ht="51.75">
+      <c r="B45" s="29"/>
+      <c r="C45" s="20">
         <v>41</v>
       </c>
-      <c r="D43" s="15" t="s">
+      <c r="D45" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="E43" s="15" t="s">
+      <c r="E45" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="F43" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G43" s="18"/>
-    </row>
-    <row r="44" spans="2:7" ht="51.75">
-      <c r="B44" s="27"/>
-      <c r="C44" s="21">
+      <c r="F45" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G45" s="17"/>
+    </row>
+    <row r="46" spans="2:7" ht="51.75">
+      <c r="B46" s="29"/>
+      <c r="C46" s="20">
         <v>42</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="D46" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="E44" s="15" t="s">
+      <c r="E46" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="F44" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G44" s="18"/>
-    </row>
-    <row r="45" spans="2:7" ht="51.75">
-      <c r="B45" s="27"/>
-      <c r="C45" s="21">
+      <c r="F46" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G46" s="17"/>
+    </row>
+    <row r="47" spans="2:7" ht="51.75">
+      <c r="B47" s="29"/>
+      <c r="C47" s="20">
         <v>43</v>
       </c>
-      <c r="D45" s="15" t="s">
+      <c r="D47" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="E45" s="15" t="s">
+      <c r="E47" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="F45" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G45" s="18"/>
-    </row>
-    <row r="46" spans="2:7" ht="51.75">
-      <c r="B46" s="27"/>
-      <c r="C46" s="21">
+      <c r="F47" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G47" s="17"/>
+    </row>
+    <row r="48" spans="2:7" ht="51.75">
+      <c r="B48" s="29"/>
+      <c r="C48" s="20">
         <v>44</v>
       </c>
-      <c r="D46" s="15" t="s">
+      <c r="D48" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="E46" s="15" t="s">
+      <c r="E48" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="F46" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G46" s="18"/>
-    </row>
-    <row r="47" spans="2:7" ht="51.75">
-      <c r="B47" s="27"/>
-      <c r="C47" s="21">
+      <c r="F48" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G48" s="17"/>
+    </row>
+    <row r="49" spans="2:7" ht="51.75">
+      <c r="B49" s="29"/>
+      <c r="C49" s="20">
         <v>45</v>
       </c>
-      <c r="D47" s="15" t="s">
+      <c r="D49" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="E47" s="15" t="s">
+      <c r="E49" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="F47" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G47" s="18"/>
-    </row>
-    <row r="48" spans="2:7" ht="64.5">
-      <c r="B48" s="27"/>
-      <c r="C48" s="21">
+      <c r="F49" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G49" s="17"/>
+    </row>
+    <row r="50" spans="2:7" ht="64.5">
+      <c r="B50" s="29"/>
+      <c r="C50" s="20">
         <v>46</v>
       </c>
-      <c r="D48" s="15" t="s">
+      <c r="D50" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="E48" s="15" t="s">
+      <c r="E50" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="F48" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G48" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" ht="64.5">
-      <c r="B49" s="27"/>
-      <c r="C49" s="21">
+      <c r="F50" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G50" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" ht="64.5">
+      <c r="B51" s="29"/>
+      <c r="C51" s="20">
         <v>47</v>
       </c>
-      <c r="D49" s="15" t="s">
+      <c r="D51" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="E49" s="15" t="s">
+      <c r="E51" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="F49" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G49" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" ht="64.5">
-      <c r="B50" s="27"/>
-      <c r="C50" s="21">
+      <c r="F51" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G51" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="64.5">
+      <c r="B52" s="29"/>
+      <c r="C52" s="20">
         <v>48</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="D52" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="E50" s="15" t="s">
+      <c r="E52" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="F50" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G50" s="18"/>
-    </row>
-    <row r="51" spans="2:7" ht="64.5">
-      <c r="B51" s="27"/>
-      <c r="C51" s="21">
+      <c r="F52" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G52" s="17"/>
+    </row>
+    <row r="53" spans="2:7" ht="64.5">
+      <c r="B53" s="29"/>
+      <c r="C53" s="20">
         <v>49</v>
       </c>
-      <c r="D51" s="15" t="s">
+      <c r="D53" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="E51" s="15" t="s">
+      <c r="E53" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="F51" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G51" s="18"/>
-    </row>
-    <row r="52" spans="2:7" ht="64.5">
-      <c r="B52" s="27"/>
-      <c r="C52" s="21">
+      <c r="F53" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G53" s="17"/>
+    </row>
+    <row r="54" spans="2:7" ht="64.5">
+      <c r="B54" s="29"/>
+      <c r="C54" s="20">
         <v>50</v>
       </c>
-      <c r="D52" s="15" t="s">
+      <c r="D54" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="E52" s="15" t="s">
+      <c r="E54" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="F52" s="18"/>
-      <c r="G52" s="18"/>
-    </row>
-    <row r="53" spans="2:7" ht="64.5">
-      <c r="B53" s="27"/>
-      <c r="C53" s="21">
+      <c r="F54" s="17"/>
+      <c r="G54" s="17"/>
+    </row>
+    <row r="55" spans="2:7" ht="64.5">
+      <c r="B55" s="29"/>
+      <c r="C55" s="20">
         <v>51</v>
       </c>
-      <c r="D53" s="15" t="s">
+      <c r="D55" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="E53" s="15" t="s">
+      <c r="E55" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="F53" s="18"/>
-      <c r="G53" s="18"/>
-    </row>
-    <row r="54" spans="2:7" ht="64.5">
-      <c r="B54" s="27"/>
-      <c r="C54" s="21">
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
+    </row>
+    <row r="56" spans="2:7" ht="64.5">
+      <c r="B56" s="29"/>
+      <c r="C56" s="20">
         <v>52</v>
       </c>
-      <c r="D54" s="15" t="s">
+      <c r="D56" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="E54" s="15" t="s">
+      <c r="E56" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="F54" s="18"/>
-      <c r="G54" s="18"/>
-    </row>
-    <row r="55" spans="2:7" ht="64.5">
-      <c r="B55" s="27"/>
-      <c r="C55" s="21">
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+    </row>
+    <row r="57" spans="2:7" ht="64.5">
+      <c r="B57" s="29"/>
+      <c r="C57" s="20">
         <v>53</v>
       </c>
-      <c r="D55" s="15" t="s">
+      <c r="D57" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="E55" s="15" t="s">
+      <c r="E57" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
-    </row>
-    <row r="56" spans="2:7" ht="51.75">
-      <c r="B56" s="27"/>
-      <c r="C56" s="21">
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
+    </row>
+    <row r="58" spans="2:7" ht="51.75">
+      <c r="B58" s="29"/>
+      <c r="C58" s="20">
         <v>54</v>
       </c>
-      <c r="D56" s="15" t="s">
+      <c r="D58" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="E56" s="15" t="s">
+      <c r="E58" s="14" t="s">
         <v>205</v>
       </c>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
-    </row>
-    <row r="57" spans="2:7" ht="51.75">
-      <c r="B57" s="27"/>
-      <c r="C57" s="21">
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
+    </row>
+    <row r="59" spans="2:7" ht="51.75">
+      <c r="B59" s="29"/>
+      <c r="C59" s="20">
         <v>55</v>
       </c>
-      <c r="D57" s="15" t="s">
+      <c r="D59" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="E57" s="15" t="s">
+      <c r="E59" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="F57" s="18"/>
-      <c r="G57" s="18"/>
-    </row>
-    <row r="58" spans="2:7" ht="51.75">
-      <c r="B58" s="27"/>
-      <c r="C58" s="21">
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+    </row>
+    <row r="60" spans="2:7" ht="51.75">
+      <c r="B60" s="29"/>
+      <c r="C60" s="20">
         <v>56</v>
       </c>
-      <c r="D58" s="15" t="s">
+      <c r="D60" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="E58" s="15" t="s">
+      <c r="E60" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="F58" s="18"/>
-      <c r="G58" s="18"/>
-    </row>
-    <row r="59" spans="2:7" ht="51.75">
-      <c r="B59" s="27"/>
-      <c r="C59" s="21">
+      <c r="F60" s="17"/>
+      <c r="G60" s="17"/>
+    </row>
+    <row r="61" spans="2:7" ht="51.75">
+      <c r="B61" s="29"/>
+      <c r="C61" s="20">
         <v>57</v>
       </c>
-      <c r="D59" s="15" t="s">
+      <c r="D61" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="E59" s="15" t="s">
+      <c r="E61" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="F59" s="18"/>
-      <c r="G59" s="18"/>
-    </row>
-    <row r="60" spans="2:7" ht="51.75">
-      <c r="B60" s="27"/>
-      <c r="C60" s="21">
+      <c r="F61" s="17"/>
+      <c r="G61" s="17"/>
+    </row>
+    <row r="62" spans="2:7" ht="51.75">
+      <c r="B62" s="29"/>
+      <c r="C62" s="20">
         <v>58</v>
       </c>
-      <c r="D60" s="15" t="s">
+      <c r="D62" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="E60" s="15" t="s">
+      <c r="E62" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="F60" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G60" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" ht="51.75">
-      <c r="B61" s="27"/>
-      <c r="C61" s="21">
+      <c r="F62" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G62" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" ht="51.75">
+      <c r="B63" s="29"/>
+      <c r="C63" s="20">
         <v>59</v>
       </c>
-      <c r="D61" s="15" t="s">
+      <c r="D63" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="E61" s="15" t="s">
+      <c r="E63" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="F61" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G61" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="62" spans="2:7" ht="51.75">
-      <c r="B62" s="27"/>
-      <c r="C62" s="21">
+      <c r="F63" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G63" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" ht="51.75">
+      <c r="B64" s="29"/>
+      <c r="C64" s="20">
         <v>60</v>
       </c>
-      <c r="D62" s="15" t="s">
+      <c r="D64" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="E62" s="15" t="s">
+      <c r="E64" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="F62" s="18"/>
-      <c r="G62" s="18"/>
-    </row>
-    <row r="63" spans="2:7" ht="51.75">
-      <c r="B63" s="27"/>
-      <c r="C63" s="21">
+      <c r="F64" s="17"/>
+      <c r="G64" s="17"/>
+    </row>
+    <row r="65" spans="2:7" ht="51.75">
+      <c r="B65" s="29"/>
+      <c r="C65" s="20">
         <v>61</v>
       </c>
-      <c r="D63" s="15" t="s">
+      <c r="D65" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="E63" s="15" t="s">
+      <c r="E65" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="F63" s="18"/>
-      <c r="G63" s="18"/>
-    </row>
-    <row r="64" spans="2:7" ht="51.75">
-      <c r="B64" s="27"/>
-      <c r="C64" s="21">
+      <c r="F65" s="17"/>
+      <c r="G65" s="17"/>
+    </row>
+    <row r="66" spans="2:7" ht="51.75">
+      <c r="B66" s="29"/>
+      <c r="C66" s="20">
         <v>62</v>
       </c>
-      <c r="D64" s="15" t="s">
+      <c r="D66" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="E64" s="15" t="s">
+      <c r="E66" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="F64" s="18"/>
-      <c r="G64" s="18"/>
-    </row>
-    <row r="65" spans="2:7" ht="51.75">
-      <c r="B65" s="27"/>
-      <c r="C65" s="21">
+      <c r="F66" s="17"/>
+      <c r="G66" s="17"/>
+    </row>
+    <row r="67" spans="2:7" ht="51.75">
+      <c r="B67" s="29"/>
+      <c r="C67" s="20">
         <v>63</v>
       </c>
-      <c r="D65" s="15" t="s">
+      <c r="D67" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="E65" s="15" t="s">
+      <c r="E67" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="F65" s="18"/>
-      <c r="G65" s="18"/>
-    </row>
-    <row r="66" spans="2:7" ht="51.75">
-      <c r="B66" s="26" t="s">
+      <c r="F67" s="17"/>
+      <c r="G67" s="17"/>
+    </row>
+    <row r="68" spans="2:7" ht="51.75">
+      <c r="B68" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="C66" s="21">
+      <c r="C68" s="20">
         <v>64</v>
       </c>
-      <c r="D66" s="19" t="s">
+      <c r="D68" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="E66" s="19" t="s">
+      <c r="E68" s="18" t="s">
         <v>180</v>
       </c>
-      <c r="F66" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G66" s="18"/>
-    </row>
-    <row r="67" spans="2:7" ht="51.75">
-      <c r="B67" s="26"/>
-      <c r="C67" s="21">
+      <c r="F68" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G68" s="17"/>
+    </row>
+    <row r="69" spans="2:7" ht="51.75">
+      <c r="B69" s="28"/>
+      <c r="C69" s="20">
         <v>65</v>
       </c>
-      <c r="D67" s="19" t="s">
+      <c r="D69" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E67" s="19" t="s">
+      <c r="E69" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="F67" s="18"/>
-      <c r="G67" s="18"/>
-    </row>
-    <row r="68" spans="2:7" ht="51.75">
-      <c r="B68" s="26"/>
-      <c r="C68" s="21">
+      <c r="F69" s="17"/>
+      <c r="G69" s="17"/>
+    </row>
+    <row r="70" spans="2:7" ht="51.75">
+      <c r="B70" s="28"/>
+      <c r="C70" s="20">
         <v>66</v>
       </c>
-      <c r="D68" s="19" t="s">
+      <c r="D70" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="E68" s="19" t="s">
+      <c r="E70" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="F68" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G68" s="18"/>
-    </row>
-    <row r="69" spans="2:7" ht="64.5">
-      <c r="B69" s="26"/>
-      <c r="C69" s="21">
+      <c r="F70" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G70" s="17"/>
+    </row>
+    <row r="71" spans="2:7" ht="64.5">
+      <c r="B71" s="28"/>
+      <c r="C71" s="20">
         <v>67</v>
       </c>
-      <c r="D69" s="19" t="s">
+      <c r="D71" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="E69" s="19" t="s">
+      <c r="E71" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="F69" s="18"/>
-      <c r="G69" s="18"/>
-    </row>
-    <row r="70" spans="2:7" ht="51.75">
-      <c r="B70" s="26"/>
-      <c r="C70" s="21">
+      <c r="F71" s="17"/>
+      <c r="G71" s="17"/>
+    </row>
+    <row r="72" spans="2:7" ht="51.75">
+      <c r="B72" s="28"/>
+      <c r="C72" s="20">
         <v>68</v>
       </c>
-      <c r="D70" s="19" t="s">
+      <c r="D72" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="E70" s="19" t="s">
+      <c r="E72" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="F70" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G70" s="18"/>
-    </row>
-    <row r="71" spans="2:7" ht="51.75">
-      <c r="B71" s="26"/>
-      <c r="C71" s="21">
+      <c r="F72" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G72" s="17"/>
+    </row>
+    <row r="73" spans="2:7" ht="51.75">
+      <c r="B73" s="28"/>
+      <c r="C73" s="20">
         <v>69</v>
       </c>
-      <c r="D71" s="19" t="s">
+      <c r="D73" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="E71" s="19" t="s">
+      <c r="E73" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="F71" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G71" s="18"/>
-    </row>
-    <row r="72" spans="2:7" ht="51.75">
-      <c r="B72" s="26"/>
-      <c r="C72" s="21">
+      <c r="F73" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G73" s="17"/>
+    </row>
+    <row r="74" spans="2:7" ht="51.75">
+      <c r="B74" s="28"/>
+      <c r="C74" s="20">
         <v>70</v>
       </c>
-      <c r="D72" s="19" t="s">
+      <c r="D74" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E72" s="19" t="s">
+      <c r="E74" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="F72" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G72" s="18"/>
-    </row>
-    <row r="73" spans="2:7" ht="39">
-      <c r="B73" s="26" t="s">
+      <c r="F74" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G74" s="17"/>
+    </row>
+    <row r="75" spans="2:7" ht="39">
+      <c r="B75" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="C73" s="21">
+      <c r="C75" s="20">
         <v>71</v>
       </c>
-      <c r="D73" s="20" t="s">
+      <c r="D75" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="E73" s="20" t="s">
+      <c r="E75" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="F73" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G73" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="74" spans="2:7" ht="39">
-      <c r="B74" s="26"/>
-      <c r="C74" s="21">
+      <c r="F75" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G75" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" ht="39">
+      <c r="B76" s="28"/>
+      <c r="C76" s="20">
         <v>72</v>
       </c>
-      <c r="D74" s="20" t="s">
+      <c r="D76" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="E74" s="20" t="s">
+      <c r="E76" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="F74" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G74" s="18"/>
-    </row>
-    <row r="75" spans="2:7" ht="39">
-      <c r="B75" s="26"/>
-      <c r="C75" s="21">
+      <c r="F76" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G76" s="17"/>
+    </row>
+    <row r="77" spans="2:7" ht="39">
+      <c r="B77" s="28"/>
+      <c r="C77" s="20">
         <v>73</v>
       </c>
-      <c r="D75" s="20" t="s">
+      <c r="D77" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="E75" s="20" t="s">
+      <c r="E77" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="F75" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G75" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="76" spans="2:7" ht="39">
-      <c r="B76" s="26"/>
-      <c r="C76" s="21">
+      <c r="F77" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G77" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" ht="39">
+      <c r="B78" s="28"/>
+      <c r="C78" s="20">
         <v>74</v>
       </c>
-      <c r="D76" s="20" t="s">
+      <c r="D78" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E76" s="20" t="s">
+      <c r="E78" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="F76" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G76" s="18"/>
-    </row>
-    <row r="77" spans="2:7" ht="51.75">
-      <c r="B77" s="26"/>
-      <c r="C77" s="21">
+      <c r="F78" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G78" s="17"/>
+    </row>
+    <row r="79" spans="2:7" ht="51.75">
+      <c r="B79" s="28"/>
+      <c r="C79" s="20">
         <v>75</v>
       </c>
-      <c r="D77" s="20" t="s">
+      <c r="D79" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="E77" s="20" t="s">
+      <c r="E79" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="F77" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G77" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="78" spans="2:7" ht="51.75">
-      <c r="B78" s="26"/>
-      <c r="C78" s="21">
+      <c r="F79" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G79" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" ht="51.75">
+      <c r="B80" s="28"/>
+      <c r="C80" s="20">
         <v>76</v>
       </c>
-      <c r="D78" s="20" t="s">
+      <c r="D80" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="E78" s="20" t="s">
+      <c r="E80" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="F78" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G78" s="18"/>
-    </row>
-    <row r="79" spans="2:7" ht="51.75">
-      <c r="B79" s="26"/>
-      <c r="C79" s="21">
+      <c r="F80" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G80" s="17"/>
+    </row>
+    <row r="81" spans="2:7" ht="51.75">
+      <c r="B81" s="28"/>
+      <c r="C81" s="20">
         <v>77</v>
       </c>
-      <c r="D79" s="20" t="s">
+      <c r="D81" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="E79" s="20" t="s">
+      <c r="E81" s="19" t="s">
         <v>254</v>
       </c>
-      <c r="F79" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G79" s="18"/>
-    </row>
-    <row r="80" spans="2:7" ht="51.75">
-      <c r="B80" s="26"/>
-      <c r="C80" s="21">
+      <c r="F81" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G81" s="17"/>
+    </row>
+    <row r="82" spans="2:7" ht="51.75">
+      <c r="B82" s="28"/>
+      <c r="C82" s="20">
         <v>78</v>
       </c>
-      <c r="D80" s="20" t="s">
+      <c r="D82" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="E80" s="20" t="s">
+      <c r="E82" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="F80" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G80" s="18"/>
-    </row>
-    <row r="81" spans="2:7" ht="39">
-      <c r="B81" s="26"/>
-      <c r="C81" s="21">
+      <c r="F82" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G82" s="17"/>
+    </row>
+    <row r="83" spans="2:7" ht="39">
+      <c r="B83" s="28"/>
+      <c r="C83" s="20">
         <v>79</v>
       </c>
-      <c r="D81" s="20" t="s">
+      <c r="D83" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E81" s="20" t="s">
+      <c r="E83" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="F81" s="18"/>
-      <c r="G81" s="18"/>
-    </row>
-    <row r="82" spans="2:7" ht="39">
-      <c r="B82" s="26"/>
-      <c r="C82" s="21">
+      <c r="F83" s="17"/>
+      <c r="G83" s="17"/>
+    </row>
+    <row r="84" spans="2:7" ht="39">
+      <c r="B84" s="28"/>
+      <c r="C84" s="20">
         <v>80</v>
       </c>
-      <c r="D82" s="20" t="s">
+      <c r="D84" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="E82" s="20" t="s">
+      <c r="E84" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="F82" s="18"/>
-      <c r="G82" s="18"/>
-    </row>
-    <row r="83" spans="2:7" ht="64.5">
-      <c r="B83" s="26"/>
-      <c r="C83" s="21">
+      <c r="F84" s="17"/>
+      <c r="G84" s="17"/>
+    </row>
+    <row r="85" spans="2:7" ht="64.5">
+      <c r="B85" s="28"/>
+      <c r="C85" s="20">
         <v>81</v>
       </c>
-      <c r="D83" s="20" t="s">
+      <c r="D85" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="E83" s="20" t="s">
+      <c r="E85" s="19" t="s">
         <v>235</v>
       </c>
-      <c r="F83" s="18"/>
-      <c r="G83" s="18"/>
-    </row>
-    <row r="84" spans="2:7" ht="64.5">
-      <c r="B84" s="26"/>
-      <c r="C84" s="21">
+      <c r="F85" s="17"/>
+      <c r="G85" s="17"/>
+    </row>
+    <row r="86" spans="2:7" ht="64.5">
+      <c r="B86" s="28"/>
+      <c r="C86" s="20">
         <v>82</v>
       </c>
-      <c r="D84" s="20" t="s">
+      <c r="D86" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E84" s="20" t="s">
+      <c r="E86" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="F84" s="18"/>
-      <c r="G84" s="18"/>
-    </row>
-    <row r="85" spans="2:7" ht="39">
-      <c r="B85" s="26"/>
-      <c r="C85" s="21">
+      <c r="F86" s="17"/>
+      <c r="G86" s="17"/>
+    </row>
+    <row r="87" spans="2:7" ht="39">
+      <c r="B87" s="28"/>
+      <c r="C87" s="20">
         <v>83</v>
       </c>
-      <c r="D85" s="20" t="s">
+      <c r="D87" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="E85" s="20" t="s">
+      <c r="E87" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="F85" s="18"/>
-      <c r="G85" s="18"/>
-    </row>
-    <row r="86" spans="2:7" ht="39">
-      <c r="B86" s="26"/>
-      <c r="C86" s="21">
+      <c r="F87" s="17"/>
+      <c r="G87" s="17"/>
+    </row>
+    <row r="88" spans="2:7" ht="39">
+      <c r="B88" s="28"/>
+      <c r="C88" s="20">
         <v>84</v>
       </c>
-      <c r="D86" s="20" t="s">
+      <c r="D88" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="E86" s="20" t="s">
+      <c r="E88" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="F86" s="18"/>
-      <c r="G86" s="18"/>
-    </row>
-    <row r="87" spans="2:7" ht="64.5">
-      <c r="B87" s="26"/>
-      <c r="C87" s="21">
+      <c r="F88" s="17"/>
+      <c r="G88" s="17"/>
+    </row>
+    <row r="89" spans="2:7" ht="64.5">
+      <c r="B89" s="28"/>
+      <c r="C89" s="20">
         <v>85</v>
       </c>
-      <c r="D87" s="20" t="s">
+      <c r="D89" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="E87" s="20" t="s">
+      <c r="E89" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="F87" s="18"/>
-      <c r="G87" s="18"/>
-    </row>
-    <row r="88" spans="2:7" ht="64.5">
-      <c r="B88" s="26"/>
-      <c r="C88" s="21">
+      <c r="F89" s="17"/>
+      <c r="G89" s="17"/>
+    </row>
+    <row r="90" spans="2:7" ht="64.5">
+      <c r="B90" s="28"/>
+      <c r="C90" s="20">
         <v>86</v>
       </c>
-      <c r="D88" s="20" t="s">
+      <c r="D90" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="E88" s="20" t="s">
+      <c r="E90" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="F88" s="18"/>
-      <c r="G88" s="18"/>
-    </row>
-    <row r="89" spans="2:7" ht="39">
-      <c r="B89" s="26"/>
-      <c r="C89" s="21">
+      <c r="F90" s="17"/>
+      <c r="G90" s="17"/>
+    </row>
+    <row r="91" spans="2:7" ht="39">
+      <c r="B91" s="28"/>
+      <c r="C91" s="20">
         <v>87</v>
       </c>
-      <c r="D89" s="20" t="s">
+      <c r="D91" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="E89" s="20" t="s">
+      <c r="E91" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="F89" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G89" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="90" spans="2:7" ht="39">
-      <c r="B90" s="26"/>
-      <c r="C90" s="21">
+      <c r="F91" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G91" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" ht="39">
+      <c r="B92" s="28"/>
+      <c r="C92" s="20">
         <v>88</v>
       </c>
-      <c r="D90" s="20" t="s">
+      <c r="D92" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="E90" s="20" t="s">
+      <c r="E92" s="19" t="s">
         <v>242</v>
       </c>
-      <c r="F90" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G90" s="18"/>
-    </row>
-    <row r="91" spans="2:7" ht="64.5">
-      <c r="B91" s="26"/>
-      <c r="C91" s="21">
+      <c r="F92" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G92" s="17"/>
+    </row>
+    <row r="93" spans="2:7" ht="64.5">
+      <c r="B93" s="28"/>
+      <c r="C93" s="20">
         <v>89</v>
       </c>
-      <c r="D91" s="20" t="s">
+      <c r="D93" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="E91" s="20" t="s">
+      <c r="E93" s="19" t="s">
         <v>243</v>
       </c>
-      <c r="F91" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G91" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="92" spans="2:7" ht="64.5">
-      <c r="B92" s="26"/>
-      <c r="C92" s="21">
+      <c r="F93" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G93" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" ht="64.5">
+      <c r="B94" s="28"/>
+      <c r="C94" s="20">
         <v>90</v>
       </c>
-      <c r="D92" s="20" t="s">
+      <c r="D94" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="E92" s="20" t="s">
+      <c r="E94" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="F92" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G92" s="18"/>
-    </row>
-    <row r="93" spans="2:7" ht="39">
-      <c r="B93" s="26"/>
-      <c r="C93" s="21">
+      <c r="F94" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G94" s="17"/>
+    </row>
+    <row r="95" spans="2:7" ht="39">
+      <c r="B95" s="28"/>
+      <c r="C95" s="20">
         <v>91</v>
       </c>
-      <c r="D93" s="20" t="s">
+      <c r="D95" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="E93" s="20" t="s">
+      <c r="E95" s="19" t="s">
         <v>245</v>
       </c>
-      <c r="F93" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G93" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="94" spans="2:7" ht="39">
-      <c r="B94" s="26"/>
-      <c r="C94" s="21">
+      <c r="F95" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G95" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" ht="39">
+      <c r="B96" s="28"/>
+      <c r="C96" s="20">
         <v>92</v>
       </c>
-      <c r="D94" s="20" t="s">
+      <c r="D96" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="E94" s="20" t="s">
+      <c r="E96" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="F94" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G94" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="95" spans="2:7" ht="64.5">
-      <c r="B95" s="26"/>
-      <c r="C95" s="21">
+      <c r="F96" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G96" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" ht="64.5">
+      <c r="B97" s="28"/>
+      <c r="C97" s="20">
         <v>93</v>
       </c>
-      <c r="D95" s="20" t="s">
+      <c r="D97" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="E95" s="20" t="s">
+      <c r="E97" s="19" t="s">
         <v>247</v>
       </c>
-      <c r="F95" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G95" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="96" spans="2:7" ht="64.5">
-      <c r="B96" s="26"/>
-      <c r="C96" s="21">
+      <c r="F97" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G97" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" ht="64.5">
+      <c r="B98" s="28"/>
+      <c r="C98" s="20">
         <v>94</v>
       </c>
-      <c r="D96" s="20" t="s">
+      <c r="D98" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="E96" s="20" t="s">
+      <c r="E98" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="F96" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G96" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="97" spans="2:7" ht="39">
-      <c r="B97" s="26"/>
-      <c r="C97" s="21">
+      <c r="F98" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G98" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" ht="39">
+      <c r="B99" s="28"/>
+      <c r="C99" s="20">
         <v>95</v>
       </c>
-      <c r="D97" s="20" t="s">
+      <c r="D99" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="E97" s="20" t="s">
+      <c r="E99" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="F97" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G97" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="98" spans="2:7" ht="39">
-      <c r="B98" s="26"/>
-      <c r="C98" s="21">
+      <c r="F99" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G99" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" ht="39">
+      <c r="B100" s="28"/>
+      <c r="C100" s="20">
         <v>96</v>
       </c>
-      <c r="D98" s="20" t="s">
+      <c r="D100" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="E98" s="20" t="s">
+      <c r="E100" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="F98" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G98" s="18"/>
-    </row>
-    <row r="99" spans="2:7" ht="64.5">
-      <c r="B99" s="26"/>
-      <c r="C99" s="21">
+      <c r="F100" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G100" s="17"/>
+    </row>
+    <row r="101" spans="2:7" ht="64.5">
+      <c r="B101" s="28"/>
+      <c r="C101" s="20">
         <v>97</v>
       </c>
-      <c r="D99" s="20" t="s">
+      <c r="D101" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E99" s="20" t="s">
+      <c r="E101" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="F99" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G99" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="100" spans="2:7" ht="64.5">
-      <c r="B100" s="26"/>
-      <c r="C100" s="21">
+      <c r="F101" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G101" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" ht="64.5">
+      <c r="B102" s="28"/>
+      <c r="C102" s="20">
         <v>98</v>
       </c>
-      <c r="D100" s="20" t="s">
+      <c r="D102" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="E100" s="20" t="s">
+      <c r="E102" s="19" t="s">
         <v>278</v>
       </c>
-      <c r="F100" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G100" s="18"/>
-    </row>
-    <row r="101" spans="2:7" ht="51.75">
-      <c r="B101" s="26"/>
-      <c r="C101" s="21">
+      <c r="F102" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G102" s="17"/>
+    </row>
+    <row r="103" spans="2:7" ht="51.75">
+      <c r="B103" s="28"/>
+      <c r="C103" s="20">
         <v>99</v>
       </c>
-      <c r="D101" s="20" t="s">
+      <c r="D103" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="E101" s="20" t="s">
+      <c r="E103" s="19" t="s">
         <v>255</v>
       </c>
-      <c r="F101" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G101" s="18"/>
-    </row>
-    <row r="102" spans="2:7" ht="51.75">
-      <c r="B102" s="26"/>
-      <c r="C102" s="21">
+      <c r="F103" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G103" s="17"/>
+    </row>
+    <row r="104" spans="2:7" ht="51.75">
+      <c r="B104" s="28"/>
+      <c r="C104" s="20">
         <v>100</v>
       </c>
-      <c r="D102" s="20" t="s">
+      <c r="D104" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="E102" s="20" t="s">
+      <c r="E104" s="19" t="s">
         <v>256</v>
       </c>
-      <c r="F102" s="18"/>
-      <c r="G102" s="18"/>
-    </row>
-    <row r="103" spans="2:7" ht="77.25">
-      <c r="B103" s="26"/>
-      <c r="C103" s="21">
+      <c r="F104" s="17"/>
+      <c r="G104" s="17"/>
+    </row>
+    <row r="105" spans="2:7" ht="77.25">
+      <c r="B105" s="28"/>
+      <c r="C105" s="20">
         <v>101</v>
       </c>
-      <c r="D103" s="20" t="s">
+      <c r="D105" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="E103" s="20" t="s">
+      <c r="E105" s="19" t="s">
         <v>257</v>
       </c>
-      <c r="F103" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G103" s="18"/>
-    </row>
-    <row r="104" spans="2:7" ht="77.25">
-      <c r="B104" s="26"/>
-      <c r="C104" s="21">
+      <c r="F105" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G105" s="17"/>
+    </row>
+    <row r="106" spans="2:7" ht="77.25">
+      <c r="B106" s="28"/>
+      <c r="C106" s="20">
         <v>102</v>
       </c>
-      <c r="D104" s="20" t="s">
+      <c r="D106" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="E104" s="20" t="s">
+      <c r="E106" s="19" t="s">
         <v>258</v>
       </c>
-      <c r="F104" s="18"/>
-      <c r="G104" s="18"/>
-    </row>
-    <row r="105" spans="2:7" ht="39">
-      <c r="B105" s="26"/>
-      <c r="C105" s="21">
+      <c r="F106" s="17"/>
+      <c r="G106" s="17"/>
+    </row>
+    <row r="107" spans="2:7" ht="39">
+      <c r="B107" s="28"/>
+      <c r="C107" s="20">
         <v>103</v>
       </c>
-      <c r="D105" s="20" t="s">
+      <c r="D107" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="E105" s="20" t="s">
+      <c r="E107" s="19" t="s">
         <v>259</v>
       </c>
-      <c r="F105" s="18"/>
-      <c r="G105" s="18"/>
-    </row>
-    <row r="106" spans="2:7" ht="39">
-      <c r="B106" s="26"/>
-      <c r="C106" s="21">
+      <c r="F107" s="17"/>
+      <c r="G107" s="17"/>
+    </row>
+    <row r="108" spans="2:7" ht="39">
+      <c r="B108" s="28"/>
+      <c r="C108" s="20">
         <v>104</v>
       </c>
-      <c r="D106" s="20" t="s">
+      <c r="D108" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="E106" s="20" t="s">
+      <c r="E108" s="19" t="s">
         <v>260</v>
       </c>
-      <c r="F106" s="18"/>
-      <c r="G106" s="18"/>
-    </row>
-    <row r="107" spans="2:7" ht="64.5">
-      <c r="B107" s="26"/>
-      <c r="C107" s="21">
+      <c r="F108" s="17"/>
+      <c r="G108" s="17"/>
+    </row>
+    <row r="109" spans="2:7" ht="64.5">
+      <c r="B109" s="28"/>
+      <c r="C109" s="20">
         <v>105</v>
       </c>
-      <c r="D107" s="20" t="s">
+      <c r="D109" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="E107" s="20" t="s">
+      <c r="E109" s="19" t="s">
         <v>261</v>
       </c>
-      <c r="F107" s="18"/>
-      <c r="G107" s="18"/>
-    </row>
-    <row r="108" spans="2:7" ht="64.5">
-      <c r="B108" s="26"/>
-      <c r="C108" s="21">
+      <c r="F109" s="17"/>
+      <c r="G109" s="17"/>
+    </row>
+    <row r="110" spans="2:7" ht="64.5">
+      <c r="B110" s="28"/>
+      <c r="C110" s="20">
         <v>106</v>
       </c>
-      <c r="D108" s="20" t="s">
+      <c r="D110" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="E108" s="20" t="s">
+      <c r="E110" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="F108" s="18"/>
-      <c r="G108" s="18"/>
-    </row>
-    <row r="109" spans="2:7" ht="39">
-      <c r="B109" s="26"/>
-      <c r="C109" s="21">
+      <c r="F110" s="17"/>
+      <c r="G110" s="17"/>
+    </row>
+    <row r="111" spans="2:7" ht="39">
+      <c r="B111" s="28"/>
+      <c r="C111" s="20">
         <v>107</v>
       </c>
-      <c r="D109" s="20" t="s">
+      <c r="D111" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="E109" s="20" t="s">
+      <c r="E111" s="19" t="s">
         <v>263</v>
       </c>
-      <c r="F109" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G109" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="110" spans="2:7" ht="39">
-      <c r="B110" s="26"/>
-      <c r="C110" s="21">
+      <c r="F111" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G111" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7" ht="39">
+      <c r="B112" s="28"/>
+      <c r="C112" s="20">
         <v>108</v>
       </c>
-      <c r="D110" s="20" t="s">
+      <c r="D112" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="E110" s="20" t="s">
+      <c r="E112" s="19" t="s">
         <v>264</v>
       </c>
-      <c r="F110" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G110" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="111" spans="2:7" ht="64.5">
-      <c r="B111" s="26"/>
-      <c r="C111" s="21">
+      <c r="F112" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G112" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7" ht="64.5">
+      <c r="B113" s="28"/>
+      <c r="C113" s="20">
         <v>109</v>
       </c>
-      <c r="D111" s="20" t="s">
+      <c r="D113" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="E111" s="20" t="s">
+      <c r="E113" s="19" t="s">
         <v>265</v>
       </c>
-      <c r="F111" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G111" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="112" spans="2:7" ht="64.5">
-      <c r="B112" s="26"/>
-      <c r="C112" s="21">
+      <c r="F113" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G113" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7" ht="64.5">
+      <c r="B114" s="28"/>
+      <c r="C114" s="20">
         <v>110</v>
       </c>
-      <c r="D112" s="20" t="s">
+      <c r="D114" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="E112" s="20" t="s">
+      <c r="E114" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="F112" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G112" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="113" spans="2:7" ht="39">
-      <c r="B113" s="26"/>
-      <c r="C113" s="21">
+      <c r="F114" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G114" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7" ht="39">
+      <c r="B115" s="28"/>
+      <c r="C115" s="20">
         <v>111</v>
       </c>
-      <c r="D113" s="20" t="s">
+      <c r="D115" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="E113" s="20" t="s">
+      <c r="E115" s="19" t="s">
         <v>267</v>
       </c>
-      <c r="F113" s="18"/>
-      <c r="G113" s="18"/>
-    </row>
-    <row r="114" spans="2:7" ht="39">
-      <c r="B114" s="26"/>
-      <c r="C114" s="21">
+      <c r="F115" s="17"/>
+      <c r="G115" s="17"/>
+    </row>
+    <row r="116" spans="2:7" ht="39">
+      <c r="B116" s="28"/>
+      <c r="C116" s="20">
         <v>112</v>
       </c>
-      <c r="D114" s="20" t="s">
+      <c r="D116" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="E114" s="20" t="s">
+      <c r="E116" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="F114" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G114" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="115" spans="2:7" ht="77.25">
-      <c r="B115" s="26"/>
-      <c r="C115" s="21">
+      <c r="F116" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G116" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="117" spans="2:7" ht="77.25">
+      <c r="B117" s="28"/>
+      <c r="C117" s="20">
         <v>113</v>
       </c>
-      <c r="D115" s="20" t="s">
+      <c r="D117" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="E115" s="20" t="s">
+      <c r="E117" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="F115" s="18"/>
-      <c r="G115" s="18"/>
-    </row>
-    <row r="116" spans="2:7" ht="77.25">
-      <c r="B116" s="26"/>
-      <c r="C116" s="21">
+      <c r="F117" s="17"/>
+      <c r="G117" s="17"/>
+    </row>
+    <row r="118" spans="2:7" ht="77.25">
+      <c r="B118" s="28"/>
+      <c r="C118" s="20">
         <v>114</v>
       </c>
-      <c r="D116" s="20" t="s">
+      <c r="D118" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="E116" s="20" t="s">
+      <c r="E118" s="19" t="s">
         <v>270</v>
       </c>
-      <c r="F116" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G116" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="117" spans="2:7" ht="39">
-      <c r="B117" s="26"/>
-      <c r="C117" s="21">
+      <c r="F118" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G118" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7" ht="39">
+      <c r="B119" s="28"/>
+      <c r="C119" s="20">
         <v>115</v>
       </c>
-      <c r="D117" s="20" t="s">
+      <c r="D119" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="E117" s="20" t="s">
+      <c r="E119" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="F117" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G117" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="118" spans="2:7" ht="39">
-      <c r="B118" s="26"/>
-      <c r="C118" s="21">
+      <c r="F119" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G119" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7" ht="39">
+      <c r="B120" s="28"/>
+      <c r="C120" s="20">
         <v>116</v>
       </c>
-      <c r="D118" s="20" t="s">
+      <c r="D120" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="E118" s="20" t="s">
+      <c r="E120" s="19" t="s">
         <v>272</v>
       </c>
-      <c r="F118" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G118" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="119" spans="2:7" ht="77.25">
-      <c r="B119" s="26"/>
-      <c r="C119" s="21">
+      <c r="F120" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G120" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="121" spans="2:7" ht="77.25">
+      <c r="B121" s="28"/>
+      <c r="C121" s="20">
         <v>117</v>
       </c>
-      <c r="D119" s="20" t="s">
+      <c r="D121" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="E119" s="20" t="s">
+      <c r="E121" s="19" t="s">
         <v>273</v>
       </c>
-      <c r="F119" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G119" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="120" spans="2:7" ht="77.25">
-      <c r="B120" s="26"/>
-      <c r="C120" s="21">
+      <c r="F121" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G121" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="122" spans="2:7" ht="77.25">
+      <c r="B122" s="28"/>
+      <c r="C122" s="20">
         <v>118</v>
       </c>
-      <c r="D120" s="20" t="s">
+      <c r="D122" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="E120" s="20" t="s">
+      <c r="E122" s="19" t="s">
         <v>274</v>
       </c>
-      <c r="F120" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G120" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="121" spans="2:7" ht="39">
-      <c r="B121" s="26"/>
-      <c r="C121" s="21">
+      <c r="F122" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G122" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7" ht="39">
+      <c r="B123" s="28"/>
+      <c r="C123" s="20">
         <v>119</v>
       </c>
-      <c r="D121" s="20" t="s">
+      <c r="D123" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="E121" s="20" t="s">
+      <c r="E123" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="F121" s="18"/>
-      <c r="G121" s="18"/>
-    </row>
-    <row r="122" spans="2:7" ht="39">
-      <c r="B122" s="26"/>
-      <c r="C122" s="21">
+      <c r="F123" s="17"/>
+      <c r="G123" s="17"/>
+    </row>
+    <row r="124" spans="2:7" ht="39">
+      <c r="B124" s="28"/>
+      <c r="C124" s="20">
         <v>120</v>
       </c>
-      <c r="D122" s="20" t="s">
+      <c r="D124" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="E122" s="20" t="s">
+      <c r="E124" s="19" t="s">
         <v>250</v>
       </c>
-      <c r="F122" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G122" s="18"/>
-    </row>
-    <row r="123" spans="2:7" ht="77.25">
-      <c r="B123" s="26"/>
-      <c r="C123" s="21">
+      <c r="F124" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G124" s="17"/>
+    </row>
+    <row r="125" spans="2:7" ht="77.25">
+      <c r="B125" s="28"/>
+      <c r="C125" s="20">
         <v>121</v>
       </c>
-      <c r="D123" s="20" t="s">
+      <c r="D125" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="E123" s="20" t="s">
+      <c r="E125" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="F123" s="18"/>
-      <c r="G123" s="18"/>
-    </row>
-    <row r="124" spans="2:7" ht="77.25">
-      <c r="B124" s="26"/>
-      <c r="C124" s="21">
+      <c r="F125" s="17"/>
+      <c r="G125" s="17"/>
+    </row>
+    <row r="126" spans="2:7" ht="77.25">
+      <c r="B126" s="28"/>
+      <c r="C126" s="20">
         <v>122</v>
       </c>
-      <c r="D124" s="20" t="s">
+      <c r="D126" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="E124" s="20" t="s">
+      <c r="E126" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="F124" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G124" s="18"/>
+      <c r="F126" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G126" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B66:B72"/>
-    <mergeCell ref="B73:B124"/>
-    <mergeCell ref="B3:B65"/>
+  <mergeCells count="5">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="B68:B74"/>
+    <mergeCell ref="B75:B126"/>
+    <mergeCell ref="B5:B67"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" scale="93" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>